<commit_message>
Fronted fixed(pair meta&file). Save meta on completion
</commit_message>
<xml_diff>
--- a/frontend_compare/metadata/metadataform.xlsx
+++ b/frontend_compare/metadata/metadataform.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="20140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="37980" yWindow="0" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -160,29 +160,99 @@
     <t>Please provide as much information as possible. Low resolution locations reduce the usability. Our recommendation is to provide either city, zip_code or longitude and latitude coordinates.</t>
   </si>
   <si>
-    <t>The date of the sample collection. Use one of the following format: YYYY-MM-DD, YYYY-MM or YYYY</t>
-  </si>
-  <si>
     <t>host</t>
   </si>
   <si>
     <t>Additional relevant details about the isolation source.</t>
   </si>
   <si>
-    <t>Information about the isolation source (i.e. blood, laboratory experiment, urine...)</t>
-  </si>
-  <si>
     <t>accession_id</t>
   </si>
   <si>
     <t>Unique identifier given to a DNA or protein sequence record to allow for tracking of different versions of that sequence record and the associated sequence over time in a single data repository (e.g. NCBI)</t>
+  </si>
+  <si>
+    <t>Information about the isolation source (i.e. blood, laboratory experiment, urine, unknown...)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The date of the sample collection. Use one of the following format: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>YYYY-MM-DD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>YYYY-MM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>YYYY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>unknown</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -269,6 +339,13 @@
       <u/>
       <sz val="14"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -427,7 +504,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -478,6 +555,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -885,7 +965,7 @@
         <v>sample_name</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="12" t="str">
         <f>'Attribute description'!$A$5</f>
@@ -948,7 +1028,7 @@
         <v>isolation_source</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S1" s="11" t="str">
         <f>'Attribute description'!$A$20</f>
@@ -989,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1000,14 +1080,15 @@
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="94.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43" customHeight="1" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -1033,13 +1114,13 @@
     </row>
     <row r="4" spans="1:3" ht="54">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43" customHeight="1">
@@ -1144,7 +1225,7 @@
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="19" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1155,25 +1236,25 @@
       <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:3" ht="24" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="18"/>
-    </row>
-    <row r="17" spans="1:3" ht="24" customHeight="1">
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:4" ht="24" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="18"/>
-    </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1">
+      <c r="B17" s="21"/>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:4" ht="24" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -1184,7 +1265,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
+    <row r="19" spans="1:4" ht="24" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
@@ -1192,10 +1273,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="43" customHeight="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="43" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -1203,12 +1284,12 @@
         <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="43" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>7</v>
@@ -1217,7 +1298,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1">
+    <row r="22" spans="1:4" ht="24" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1228,7 +1309,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
+    <row r="23" spans="1:4" ht="24" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1320,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43" customHeight="1">
+    <row r="24" spans="1:4" ht="43" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>31</v>
       </c>
@@ -1247,10 +1328,11 @@
         <v>7</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="24" customHeight="1">
+        <v>49</v>
+      </c>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4" ht="24" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
@@ -1261,7 +1343,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="24" customHeight="1">
+    <row r="26" spans="1:4" ht="24" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>

</xml_diff>